<commit_message>
Contemplar credenciales no validas
</commit_message>
<xml_diff>
--- a/Datos/Datos_IniciarSesion.xlsx
+++ b/Datos/Datos_IniciarSesion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Practicas_Testing\Selenenium_WebDriver\sauceDemo\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE1282B-8203-40D6-A6B0-770DABB0F8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ADE84A-F915-4A17-9DEF-DBEABE51855A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7B58D147-3486-4022-A001-FE536626475D}"/>
   </bookViews>
@@ -36,21 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
   </si>
   <si>
     <t>performance_glitch_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>problem_user</t>
   </si>
 </sst>
 </file>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6044AC1A-6A6F-471E-BABC-226DD4B4820A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,40 +415,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="correo03@gmail.com" xr:uid="{63880FA2-E9D7-48F4-A862-26D4782DDC6E}"/>
-    <hyperlink ref="A1" r:id="rId2" display="correo01@gmail.com" xr:uid="{565F2968-E7C4-4AB1-9517-B31D5C42C6B8}"/>
-    <hyperlink ref="A2" r:id="rId3" display="correo02@gmail.com" xr:uid="{E5BB5661-F627-4C6D-97F2-63D0BA15DE53}"/>
+    <hyperlink ref="A1" r:id="rId1" display="correo01@gmail.com" xr:uid="{565F2968-E7C4-4AB1-9517-B31D5C42C6B8}"/>
+    <hyperlink ref="A2" r:id="rId2" display="correo02@gmail.com" xr:uid="{E5BB5661-F627-4C6D-97F2-63D0BA15DE53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>